<commit_message>
update all files and code
update as of July 31, 2023. includes everything done on IODP Expedition 399 and afterwards until this date
</commit_message>
<xml_diff>
--- a/outputs/HFResultsSummary.xlsx
+++ b/outputs/HFResultsSummary.xlsx
@@ -13,54 +13,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Cruise</t>
   </si>
   <si>
-    <t>Tutorial Cruise</t>
+    <t>chinook-TEST</t>
   </si>
   <si>
     <t>Station</t>
   </si>
   <si>
-    <t>0</t>
+    <t>HF3</t>
   </si>
   <si>
     <t>Penetration</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Trial</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>Trial</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Iterations</t>
   </si>
   <si>
     <t>10</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
     <t>Use HP?</t>
   </si>
   <si>
-    <t>Used (600 J/m)</t>
+    <t>Used (450 J/m)</t>
   </si>
   <si>
     <t>Bottom Water (°C)</t>
   </si>
   <si>
-    <t>2.555</t>
+    <t>1.7962</t>
   </si>
   <si>
     <t>Tot Sensors</t>
@@ -75,40 +69,31 @@
     <t>Tilt (°)</t>
   </si>
   <si>
-    <t>2.4</t>
+    <t>4.7</t>
   </si>
   <si>
     <t>Therm. Gradient (°C/m)</t>
   </si>
   <si>
-    <t>0.064</t>
+    <t>0.171</t>
   </si>
   <si>
     <t>Av. Therm. Conductivity (W/m°C)</t>
   </si>
   <si>
-    <t>1.101</t>
-  </si>
-  <si>
-    <t>1.126</t>
+    <t>1.353</t>
   </si>
   <si>
     <t>Heat Flow (mW/m^2)</t>
   </si>
   <si>
-    <t>68</t>
-  </si>
-  <si>
-    <t>69</t>
+    <t>230</t>
   </si>
   <si>
     <t>Shift</t>
   </si>
   <si>
-    <t>0.28</t>
-  </si>
-  <si>
-    <t>0.32</t>
+    <t>0.15</t>
   </si>
   <si>
     <t>Notes</t>
@@ -157,15 +142,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O2"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="true"/>
+    <col min="1" max="1" width="6.7109375" customWidth="true"/>
     <col min="2" max="2" width="7.42578125" customWidth="true"/>
     <col min="3" max="3" width="11.7109375" customWidth="true"/>
     <col min="4" max="4" width="5" customWidth="true"/>
     <col min="5" max="5" width="9.7109375" customWidth="true"/>
-    <col min="6" max="6" width="14.140625" customWidth="true"/>
+    <col min="6" max="6" width="8.28515625" customWidth="true"/>
     <col min="7" max="7" width="17.28515625" customWidth="true"/>
     <col min="8" max="8" width="11.28515625" customWidth="true"/>
     <col min="9" max="9" width="15.28515625" customWidth="true"/>
@@ -191,37 +176,37 @@
         <v>6</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="0" t="s">
-        <v>18</v>
-      </c>
       <c r="J1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="L1" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="M1" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="0" t="s">
-        <v>26</v>
-      </c>
       <c r="N1" s="0" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
@@ -238,77 +223,34 @@
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>17</v>
       </c>
       <c r="I2" s="0"/>
       <c r="J2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="L2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="M2" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="0" t="s">
-        <v>27</v>
-      </c>
       <c r="N2" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="O2" s="0"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="0"/>
-      <c r="J3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="O3" s="0"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>